<commit_message>
add headers, testpads, current sense resistors, led
</commit_message>
<xml_diff>
--- a/EntireBoard/BOM.xlsx
+++ b/EntireBoard/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhiyangzhang/Desktop/NeuralRecorder/EntireBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5749A381-3E64-0B46-B3D6-75FDE9C5D7B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C8F607-7A94-D84F-86B6-6FE1C85BB16D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="460" windowWidth="18980" windowHeight="14480" xr2:uid="{CB31685E-8979-C24C-AC40-0D6B15E33466}"/>
+    <workbookView xWindow="2380" yWindow="460" windowWidth="23140" windowHeight="14460" xr2:uid="{CB31685E-8979-C24C-AC40-0D6B15E33466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -123,6 +123,75 @@
   </si>
   <si>
     <t>connection btw XDS110 and CC</t>
+  </si>
+  <si>
+    <t>current sense resistor</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>667-ERJ-MFBAF10MX</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/ERJ-MFBAF10MX?qs=sGAEpiMZZMtlleCFQhR%2fzRH%2fPnzm6Qg0kawuZXKFDVkf2mAFMVBMuA%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/315/RDN0000C328-1365505.pdf</t>
+  </si>
+  <si>
+    <t>749-SM0402GC</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bivar/SM0402GC?qs=sGAEpiMZZMsl8UZd3ZuU6aAY3C3HMTrKStrc3C%252bshI%2fhhMFkdt6RXA%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/50/Bivar-3-22-2017-SM0402GC-1158932.pdf</t>
+  </si>
+  <si>
+    <t>green led</t>
+  </si>
+  <si>
+    <t>measure power consumption</t>
+  </si>
+  <si>
+    <t>Bivar SM0402GC</t>
+  </si>
+  <si>
+    <t>Panasonic ERJ-MFBAF10MX</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>for resetting mcu</t>
+  </si>
+  <si>
+    <t>1188E-1K2-V-T/R</t>
+  </si>
+  <si>
+    <t>113-1188E1K2VTR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diptronics/1188E-1K2-V-T-R?qs=MLItCLRbWswadUUxegNFmg%3D%3D</t>
+  </si>
+  <si>
+    <t>http://www.dip.com.tw/en/en-product-information/en-switch004/item/2445-1188</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samtec-inc/FFSD-05-D-02.00-01-N/SAM8217-ND/1106576</t>
+  </si>
+  <si>
+    <t>http://suddendocs.samtec.com/catalog_english/ffsd.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samtek FFSD-05-D-02.00-01-N	</t>
+  </si>
+  <si>
+    <t>SAM8217-ND</t>
+  </si>
+  <si>
+    <t>signal line indication</t>
   </si>
 </sst>
 </file>
@@ -130,9 +199,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,19 +211,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -185,21 +266,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,26 +599,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA42242D-18CC-8D43-891A-AE4354601FB0}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
     <col min="7" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -549,7 +634,7 @@
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -565,94 +650,200 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="46" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" ht="46">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="8">
         <v>0.86</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:10" ht="34">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="7">
         <v>0.41</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="7">
         <v>3.36</v>
       </c>
-      <c r="I4" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="10">
+        <v>7.86</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.61</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.69</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quantity change to BOM
</commit_message>
<xml_diff>
--- a/EntireBoard/BOM.xlsx
+++ b/EntireBoard/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\NeuralRecorder\EntireBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhiyangzhang/Desktop/NeuralRecorder/EntireBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AED109-6E89-41F9-8F4E-F4093AE95328}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906E2F3C-6BEE-3C4A-A9A9-0D436895C097}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="460" windowWidth="21280" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -234,6 +233,7 @@
         <sz val="12"/>
         <color indexed="12"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/BLM18HE152SN1D/490-5216-1-ND/1948392</t>
     </r>
@@ -254,6 +254,7 @@
         <sz val="12"/>
         <color indexed="13"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL05A226MQ5N6J8/1276-7090-1-ND/7320732</t>
     </r>
@@ -274,6 +275,7 @@
         <sz val="12"/>
         <color indexed="12"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/500R07S1R8BV4T/712-1271-1-ND/1786733</t>
     </r>
@@ -294,6 +296,7 @@
         <sz val="12"/>
         <color indexed="12"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.digikey.com/product-detail/en/kemet/C0402C120J5GACTU/399-1013-1-ND/411288</t>
     </r>
@@ -314,6 +317,7 @@
         <sz val="12"/>
         <color indexed="12"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/500R07S1R0BV4T/712-1266-1-ND/1786728</t>
     </r>
@@ -334,6 +338,7 @@
         <sz val="12"/>
         <color indexed="12"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.digikey.com/product-detail/en/abracon-llc/AIML-0603-6R8K-T/535-11606-1-ND/2782848</t>
     </r>
@@ -354,6 +359,7 @@
         <sz val="12"/>
         <color indexed="12"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.mouser.com/ProductDetail/TDK/MHQ0603P2N0BTD25?qs=sGAEpiMZZMukHu%252bjC5l7YWgkXgROw64Zk51RBDRudIE%3d</t>
     </r>
@@ -374,6 +380,7 @@
         <sz val="12"/>
         <color indexed="12"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/LQP03TN2N4B02D/490-6724-1-ND/5802372</t>
     </r>
@@ -397,12 +404,14 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -413,23 +422,27 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color indexed="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color indexed="13"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
       <color indexed="15"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -601,9 +614,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -653,6 +663,7 @@
     <xf numFmtId="165" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1816,10 +1827,10 @@
   <dimension ref="A1:IV18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16.649999999999999" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="1" customWidth="1"/>
@@ -1833,7 +1844,7 @@
     <col min="11" max="256" width="10.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.649999999999999" customHeight="1">
+    <row r="1" spans="1:10" ht="16.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1885,9 +1896,12 @@
         <v>0.86</v>
       </c>
       <c r="G2" s="10">
-        <v>1</v>
-      </c>
-      <c r="H2" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="H2" s="39">
+        <f>F2*G2</f>
+        <v>1.72</v>
+      </c>
       <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
@@ -1915,9 +1929,12 @@
         <v>0.41</v>
       </c>
       <c r="G3" s="15">
-        <v>1</v>
-      </c>
-      <c r="H3" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="H3" s="39">
+        <f t="shared" ref="H3:H18" si="0">F3*G3</f>
+        <v>0.82</v>
+      </c>
       <c r="I3" s="11" t="s">
         <v>21</v>
       </c>
@@ -1925,7 +1942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.649999999999999" customHeight="1">
+    <row r="4" spans="1:10" ht="16.75" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
@@ -1945,9 +1962,12 @@
         <v>3.36</v>
       </c>
       <c r="G4" s="15">
-        <v>1</v>
-      </c>
-      <c r="H4" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="H4" s="39">
+        <f t="shared" si="0"/>
+        <v>6.72</v>
+      </c>
       <c r="I4" s="11" t="s">
         <v>27</v>
       </c>
@@ -1955,7 +1975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16.649999999999999" customHeight="1">
+    <row r="5" spans="1:10" ht="16.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
@@ -1977,7 +1997,10 @@
       <c r="G5" s="15">
         <v>1</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="39">
+        <f t="shared" si="0"/>
+        <v>7.86</v>
+      </c>
       <c r="I5" s="11" t="s">
         <v>33</v>
       </c>
@@ -2007,7 +2030,10 @@
       <c r="G6" s="15">
         <v>2</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="39">
+        <f t="shared" si="0"/>
+        <v>1.22</v>
+      </c>
       <c r="I6" s="11" t="s">
         <v>40</v>
       </c>
@@ -2015,7 +2041,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16.649999999999999" customHeight="1">
+    <row r="7" spans="1:10" ht="16.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
@@ -2037,7 +2063,10 @@
       <c r="G7" s="15">
         <v>6</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="39">
+        <f t="shared" si="0"/>
+        <v>3.42</v>
+      </c>
       <c r="I7" s="11" t="s">
         <v>46</v>
       </c>
@@ -2065,9 +2094,12 @@
         <v>0.69</v>
       </c>
       <c r="G8" s="15">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="H8" s="39">
+        <f t="shared" si="0"/>
+        <v>1.38</v>
+      </c>
       <c r="I8" s="11" t="s">
         <v>52</v>
       </c>
@@ -2075,7 +2107,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.4" customHeight="1">
+    <row r="9" spans="1:10" ht="15.5" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>54</v>
       </c>
@@ -2097,8 +2129,8 @@
       <c r="G9" s="20">
         <v>2</v>
       </c>
-      <c r="H9" s="20">
-        <f>34.13*2</f>
+      <c r="H9" s="39">
+        <f t="shared" si="0"/>
         <v>68.260000000000005</v>
       </c>
       <c r="I9" s="11" t="s">
@@ -2106,7 +2138,7 @@
       </c>
       <c r="J9" s="15"/>
     </row>
-    <row r="10" spans="1:10" ht="15.4" customHeight="1">
+    <row r="10" spans="1:10" ht="15.5" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>59</v>
       </c>
@@ -2128,14 +2160,14 @@
       <c r="G10" s="20">
         <v>4</v>
       </c>
-      <c r="H10" s="20">
-        <f>0.98*4</f>
+      <c r="H10" s="39">
+        <f t="shared" si="0"/>
         <v>3.92</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="1:10" ht="16.649999999999999" customHeight="1">
+    <row r="11" spans="1:10" ht="16.75" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>62</v>
       </c>
@@ -2157,7 +2189,8 @@
       <c r="G11" s="20">
         <v>1</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="39">
+        <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
       <c r="I11" s="11" t="s">
@@ -2165,131 +2198,146 @@
       </c>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="1:10" ht="22.65" customHeight="1">
+    <row r="12" spans="1:10" ht="22.75" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="24">
         <v>0.57999999999999996</v>
       </c>
       <c r="G12" s="20">
         <v>2</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="39">
+        <f t="shared" si="0"/>
+        <v>1.1599999999999999</v>
+      </c>
       <c r="I12" s="11" t="s">
         <v>70</v>
       </c>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="1:10" ht="22.65" customHeight="1">
+    <row r="13" spans="1:10" ht="22.75" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="28">
         <v>0.21</v>
       </c>
       <c r="G13" s="20">
         <v>1</v>
       </c>
-      <c r="H13" s="23"/>
+      <c r="H13" s="39">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
       <c r="I13" s="11" t="s">
         <v>74</v>
       </c>
       <c r="J13" s="15"/>
     </row>
-    <row r="14" spans="1:10" ht="22.65" customHeight="1">
+    <row r="14" spans="1:10" ht="22.75" customHeight="1">
       <c r="A14" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="31">
         <v>0.1</v>
       </c>
       <c r="G14" s="20">
         <v>4</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="39">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
       <c r="I14" s="11" t="s">
         <v>78</v>
       </c>
       <c r="J14" s="15"/>
     </row>
-    <row r="15" spans="1:10" ht="22.65" customHeight="1">
+    <row r="15" spans="1:10" ht="22.75" customHeight="1">
       <c r="A15" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="31">
         <v>0.21</v>
       </c>
       <c r="G15" s="20">
         <v>3</v>
       </c>
-      <c r="H15" s="23"/>
+      <c r="H15" s="39">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
       <c r="I15" s="11" t="s">
         <v>82</v>
       </c>
       <c r="J15" s="15"/>
     </row>
-    <row r="16" spans="1:10" ht="22.65" customHeight="1">
+    <row r="16" spans="1:10" ht="22.75" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34" t="s">
+      <c r="B16" s="32"/>
+      <c r="C16" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F16" s="35">
         <v>0.1</v>
       </c>
       <c r="G16" s="20">
         <v>1</v>
       </c>
-      <c r="H16" s="23"/>
+      <c r="H16" s="39">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
       <c r="I16" s="11" t="s">
         <v>86</v>
       </c>
@@ -2300,48 +2348,54 @@
         <v>87</v>
       </c>
       <c r="B17" s="15"/>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F17" s="35">
         <v>0.6</v>
       </c>
       <c r="G17" s="20">
         <v>2</v>
       </c>
-      <c r="H17" s="23"/>
+      <c r="H17" s="39">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
       <c r="I17" s="11" t="s">
         <v>90</v>
       </c>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="1:10" ht="22.65" customHeight="1">
+    <row r="18" spans="1:10" ht="22.75" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="15"/>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="38">
         <v>0.1</v>
       </c>
       <c r="G18" s="20">
         <v>2</v>
       </c>
-      <c r="H18" s="23"/>
+      <c r="H18" s="39">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="I18" s="11" t="s">
         <v>94</v>
       </c>

</xml_diff>